<commit_message>
Added fuction to convert backslashes to for slashes -> 0.0_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
</commit_message>
<xml_diff>
--- a/0.0_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
+++ b/0.0_Description_4_media_key_messages_&_captions/1.0_key_messages_&_captions.xlsx
@@ -5,22 +5,34 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\0.1_GitHub\1.0_Description_4_media_key_messages_&amp;_captions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\0.1_GitHub\0.0_Description_4_media_key_messages_&amp;_captions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF394B8A-16C3-4D17-82C3-ED252B044EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A061D3-3214-460B-BFB0-E47B5F501E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key_messages_&amp;_captiosn" sheetId="2" r:id="rId1"/>
     <sheet name="recording steps and topics" sheetId="4" r:id="rId2"/>
-    <sheet name="pip" sheetId="3" r:id="rId3"/>
+    <sheet name="Slach converter &amp; commints" sheetId="5" r:id="rId3"/>
+    <sheet name="pip" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -49,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>key_messages</t>
   </si>
@@ -246,6 +258,18 @@
   </si>
   <si>
     <t>llms, hugging face,Dedicated Inference Endpoint</t>
+  </si>
+  <si>
+    <t>Backslash path</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>C:\Users\Sicaja\Desktop\SmartCodeACADEMY\0.0_Channel_topics\2025.03.22-GitHub_AI_Marketing_Generator\0.1_GitHub</t>
+  </si>
+  <si>
+    <t>Add key messages, captions, and product DB; update app.py  model  to Mistral and added template of the  README</t>
   </si>
 </sst>
 </file>
@@ -345,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,6 +415,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,12 +764,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA82D05-3B3C-41E0-860A-3A51304EF733}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,6 +1083,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80838B4-7FF7-4A54-BF52-AC4F2521D054}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="207.85546875" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>SUBSTITUTE(B1, "\", "/")</f>
+        <v>C:/Users/Sicaja/Desktop/SmartCodeACADEMY/0.0_Channel_topics/2025.03.22-GitHub_AI_Marketing_Generator/0.1_GitHub</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5126FC2-5C16-47A1-BFE8-236554BE31B0}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>